<commit_message>
Added function for CLPT
</commit_message>
<xml_diff>
--- a/MATLAB/Structures/HW5_P1_InputFile.xlsx
+++ b/MATLAB/Structures/HW5_P1_InputFile.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\SE142&amp;253A\2020\HW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Stuff\Triton UAS\CarbonCopy\carbon-copy\MATLAB\Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E09CB1-3613-42CF-ACBC-1300FC1A1A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="636" windowWidth="14298" windowHeight="9348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11952" windowHeight="5916"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -214,7 +213,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -378,7 +377,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B68FA1-C050-4158-AE32-4674192698D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5B68FA1-C050-4158-AE32-4674192698D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -433,7 +432,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA2524B9-3630-47E5-9C23-C133880E2C80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AA2524B9-3630-47E5-9C23-C133880E2C80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -488,7 +487,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDFB9804-83B6-4603-A040-EFA83D3598DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FDFB9804-83B6-4603-A040-EFA83D3598DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -543,7 +542,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A22436FC-33B0-4F79-A8C6-7A786BA33BC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A22436FC-33B0-4F79-A8C6-7A786BA33BC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -598,7 +597,7 @@
         <xdr:cNvPr id="6" name="TextBox 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4007421A-8019-4A8F-BAF7-07154C0702C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4007421A-8019-4A8F-BAF7-07154C0702C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -653,7 +652,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EDB44CB-BDCF-44BA-843E-645724F5C7AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EDB44CB-BDCF-44BA-843E-645724F5C7AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -708,7 +707,7 @@
         <xdr:cNvPr id="8" name="TextBox 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0236D24-77B3-4AD3-9058-F043CD128757}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0236D24-77B3-4AD3-9058-F043CD128757}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -763,7 +762,7 @@
         <xdr:cNvPr id="9" name="TextBox 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9809854A-9364-4B94-9767-F0CCD8264386}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9809854A-9364-4B94-9767-F0CCD8264386}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -818,7 +817,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F6BB5D4-F557-4CCE-827C-AF27C747BD1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F6BB5D4-F557-4CCE-827C-AF27C747BD1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,7 +872,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33ECDDA4-8666-4298-B4C4-B183BC3071A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{33ECDDA4-8666-4298-B4C4-B183BC3071A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -928,7 +927,7 @@
         <xdr:cNvPr id="12" name="TextBox 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E2E88F2-9DDC-4D5A-AFA8-0C351C77B7AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5E2E88F2-9DDC-4D5A-AFA8-0C351C77B7AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -983,7 +982,7 @@
         <xdr:cNvPr id="13" name="TextBox 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F015E5-96E9-4458-B062-2430B80032D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{76F015E5-96E9-4458-B062-2430B80032D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1038,7 +1037,7 @@
         <xdr:cNvPr id="14" name="TextBox 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{349DB594-B73D-4C7D-B804-61FEE3918592}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{349DB594-B73D-4C7D-B804-61FEE3918592}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1093,7 +1092,7 @@
         <xdr:cNvPr id="15" name="TextBox 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380309E0-AF0F-448B-9BF5-1DE21620367F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{380309E0-AF0F-448B-9BF5-1DE21620367F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1148,7 +1147,7 @@
         <xdr:cNvPr id="16" name="TextBox 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B43DF324-94FA-40A4-B6AE-5F3029C5244F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B43DF324-94FA-40A4-B6AE-5F3029C5244F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1203,7 +1202,7 @@
         <xdr:cNvPr id="17" name="TextBox 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF3570DC-6AF1-48FD-95F7-57AE2FEB572F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CF3570DC-6AF1-48FD-95F7-57AE2FEB572F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1258,7 +1257,7 @@
         <xdr:cNvPr id="18" name="TextBox 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F6E4007-3C42-409C-9A23-149BAB65FD47}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F6E4007-3C42-409C-9A23-149BAB65FD47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1313,7 +1312,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58B1AEFC-5617-4D55-AEBB-1C303A512650}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{58B1AEFC-5617-4D55-AEBB-1C303A512650}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1368,7 +1367,7 @@
         <xdr:cNvPr id="20" name="TextBox 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1175571-E95B-46C2-974A-4543DF26A18A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C1175571-E95B-46C2-974A-4543DF26A18A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1423,7 +1422,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EED06B95-CC34-4EB3-BD46-3F1389DD249A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EED06B95-CC34-4EB3-BD46-3F1389DD249A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1478,7 +1477,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88772AB6-D941-4896-9981-4EE26EED3399}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88772AB6-D941-4896-9981-4EE26EED3399}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1533,7 +1532,7 @@
         <xdr:cNvPr id="23" name="TextBox 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4652669D-59C1-4E9D-86EA-1573B2563E66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4652669D-59C1-4E9D-86EA-1573B2563E66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1588,7 +1587,7 @@
         <xdr:cNvPr id="24" name="TextBox 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AA7AD3-AB1B-4440-9F04-1F938C3E11C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1AA7AD3-AB1B-4440-9F04-1F938C3E11C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1643,7 +1642,7 @@
         <xdr:cNvPr id="25" name="TextBox 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A95D0B-1DAC-4D90-AFD3-383811BD740A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27A95D0B-1DAC-4D90-AFD3-383811BD740A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1698,7 +1697,7 @@
         <xdr:cNvPr id="26" name="TextBox 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C9B6AF0-7CBC-45C2-9040-4C6E617D1A7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C9B6AF0-7CBC-45C2-9040-4C6E617D1A7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1753,7 +1752,7 @@
         <xdr:cNvPr id="27" name="TextBox 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB628EB0-77A0-4F2A-B4EE-C3BD1DC42383}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB628EB0-77A0-4F2A-B4EE-C3BD1DC42383}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1808,7 +1807,7 @@
         <xdr:cNvPr id="28" name="TextBox 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{958A32B4-95C7-4BFC-ABDA-920E0DF93048}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{958A32B4-95C7-4BFC-ABDA-920E0DF93048}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1863,7 +1862,7 @@
         <xdr:cNvPr id="29" name="TextBox 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB65835D-BCED-4375-B37C-F76229379D92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DB65835D-BCED-4375-B37C-F76229379D92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1918,7 +1917,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41737B1A-7485-42BD-A823-ADB97FF9E6E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{41737B1A-7485-42BD-A823-ADB97FF9E6E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1973,7 +1972,7 @@
         <xdr:cNvPr id="31" name="TextBox 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06E2A0A0-F8CF-42DD-B133-79AFE09762C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{06E2A0A0-F8CF-42DD-B133-79AFE09762C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2280,10 +2279,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
@@ -2292,7 +2293,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.8">
+    <row r="2" spans="1:13" ht="15.6">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2461,7 +2462,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14.7">
+    <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>